<commit_message>
paper work, thesis v0.8
</commit_message>
<xml_diff>
--- a/paper_work/masters thesis/msc_worktime.xlsx
+++ b/paper_work/masters thesis/msc_worktime.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44D96E4B-B62F-43DA-AEB3-D676AEFFF61D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E993727-1191-421A-9416-BAF9365EF094}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Время извлечения текста</t>
   </si>
@@ -42,24 +42,6 @@
     <t>Общее время обработки</t>
   </si>
   <si>
-    <t>Файл 1</t>
-  </si>
-  <si>
-    <t>Файл 2</t>
-  </si>
-  <si>
-    <t>Файл 3</t>
-  </si>
-  <si>
-    <t>Файл 4</t>
-  </si>
-  <si>
-    <t>Файл 5</t>
-  </si>
-  <si>
-    <t>Файл 6</t>
-  </si>
-  <si>
     <t>Количество символов</t>
   </si>
   <si>
@@ -70,13 +52,23 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="169" formatCode="0.0000"/>
+  </numFmts>
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
     </font>
   </fonts>
   <fills count="2">
@@ -99,10 +91,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="16" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="9"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -171,10 +167,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.17787051618547678"/>
-          <c:y val="0.20916666666666667"/>
-          <c:w val="0.74219213958946273"/>
-          <c:h val="0.61766987459900846"/>
+          <c:x val="0.1558319342313616"/>
+          <c:y val="0.19328735034324698"/>
+          <c:w val="0.78074662154833951"/>
+          <c:h val="0.63354905703195286"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -222,58 +218,148 @@
             </c:spPr>
             <c:trendlineType val="linear"/>
             <c:dispRSqr val="0"/>
-            <c:dispEq val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$7</c:f>
+              <c:f>Sheet1!$B$2:$B$17</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="16"/>
                 <c:pt idx="0">
                   <c:v>158.12</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>293.79000000000002</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="2" formatCode="General">
+                  <c:v>427.51</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>702.12</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4" formatCode="General">
+                  <c:v>939.52</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>1654.55</c:v>
                 </c:pt>
-                <c:pt idx="4">
-                  <c:v>9738.32</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>42533.51</c:v>
+                <c:pt idx="6" formatCode="General">
+                  <c:v>1905.22</c:v>
+                </c:pt>
+                <c:pt idx="7" formatCode="General">
+                  <c:v>2140.2600000000002</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="General">
+                  <c:v>2418.71</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="General">
+                  <c:v>2700.42</c:v>
+                </c:pt>
+                <c:pt idx="10" formatCode="General">
+                  <c:v>4209.57</c:v>
+                </c:pt>
+                <c:pt idx="11" formatCode="General">
+                  <c:v>4769.96</c:v>
+                </c:pt>
+                <c:pt idx="12" formatCode="General">
+                  <c:v>6046.34</c:v>
+                </c:pt>
+                <c:pt idx="13" formatCode="General">
+                  <c:v>7286.54</c:v>
+                </c:pt>
+                <c:pt idx="14" formatCode="General">
+                  <c:v>8746.08</c:v>
+                </c:pt>
+                <c:pt idx="15" formatCode="General">
+                  <c:v>10575.51</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$D$2:$D$7</c:f>
+              <c:f>Sheet1!$D$2:$D$17</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="16"/>
                 <c:pt idx="0">
                   <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>111</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="2" formatCode="General">
+                  <c:v>653</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>206</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4" formatCode="General">
+                  <c:v>237</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>841</c:v>
                 </c:pt>
-                <c:pt idx="4">
-                  <c:v>14437</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>35778</c:v>
+                <c:pt idx="6" formatCode="General">
+                  <c:v>762</c:v>
+                </c:pt>
+                <c:pt idx="7" formatCode="General">
+                  <c:v>610</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="General">
+                  <c:v>690</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="General">
+                  <c:v>273</c:v>
+                </c:pt>
+                <c:pt idx="10" formatCode="General">
+                  <c:v>743</c:v>
+                </c:pt>
+                <c:pt idx="11" formatCode="General">
+                  <c:v>1331</c:v>
+                </c:pt>
+                <c:pt idx="12" formatCode="General">
+                  <c:v>841</c:v>
+                </c:pt>
+                <c:pt idx="13" formatCode="General">
+                  <c:v>1322</c:v>
+                </c:pt>
+                <c:pt idx="14" formatCode="General">
+                  <c:v>1167</c:v>
+                </c:pt>
+                <c:pt idx="15" formatCode="General">
+                  <c:v>2554</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -300,7 +386,7 @@
         <c:axId val="672950608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="45000"/>
+          <c:max val="11000"/>
           <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -414,7 +500,7 @@
         <c:crossAx val="680596160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
-        <c:majorUnit val="10000"/>
+        <c:majorUnit val="2000"/>
       </c:valAx>
       <c:valAx>
         <c:axId val="680596160"/>
@@ -464,6 +550,14 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="2.2270753345914406E-2"/>
+              <c:y val="0.2088236452512133"/>
+            </c:manualLayout>
+          </c:layout>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -601,469 +695,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1440" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout>
-        <c:manualLayout>
-          <c:layoutTarget val="inner"/>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="0.15927826750739824"/>
-          <c:y val="0.20916666666666667"/>
-          <c:w val="0.77236189101860275"/>
-          <c:h val="0.61766987459900846"/>
-        </c:manualLayout>
-      </c:layout>
-      <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:v>Зависимость времени извлечения текста от размера файла</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="linear"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="0"/>
-          </c:trendline>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Sheet1!$B$2:$B$5</c:f>
-              <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>158.12</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>293.79000000000002</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>702.12</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1654.55</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Sheet1!$D$2:$D$5</c:f>
-              <c:numCache>
-                <c:formatCode>0</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>80</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>111</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>206</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>841</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-5A1F-460C-A950-484ACE2EF229}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="672950608"/>
-        <c:axId val="680596160"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="672950608"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-          <c:max val="1800"/>
-          <c:min val="0"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="ru-RU"/>
-                  <a:t>Размер файла, КБайт</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="0.00" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="680596160"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-        <c:majorUnit val="400"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="680596160"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-          <c:min val="0"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="ru-RU"/>
-                  <a:t>Время извлечения текста, мс</a:t>
-                </a:r>
-                <a:endParaRPr lang="en-US"/>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout>
-            <c:manualLayout>
-              <c:xMode val="edge"/>
-              <c:yMode val="edge"/>
-              <c:x val="1.6905396785561168E-2"/>
-              <c:y val="0.20916666666666667"/>
-            </c:manualLayout>
-          </c:layout>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="0" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="672950608"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr sz="1200"/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
       <c:tx>
         <c:rich>
           <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
@@ -1084,7 +715,15 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="ru-RU"/>
-              <a:t>Зависимость времени извлечения текста от количества</a:t>
+              <a:t>Зависимость времени работы</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="ru-RU" baseline="0"/>
+              <a:t> </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="ru-RU"/>
+              <a:t>от количества</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="ru-RU" baseline="0"/>
@@ -1130,10 +769,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.17787051618547678"/>
-          <c:y val="0.20916666666666667"/>
-          <c:w val="0.77168503937007871"/>
-          <c:h val="0.61766987459900846"/>
+          <c:x val="0.12965251985011308"/>
+          <c:y val="6.6505504393462533E-2"/>
+          <c:w val="0.83864936694233971"/>
+          <c:h val="0.49470206739392208"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -1143,7 +782,7 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>Зависимость времени извлечения текста от размера файла</c:v>
+            <c:v>Зависимость времени извлечения текста от количества страниц</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
@@ -1169,12 +808,26 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$I$2:$I$7</c:f>
+              <c:f>Sheet1!$H$18:$H$33</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="16"/>
                 <c:pt idx="0">
                   <c:v>4</c:v>
                 </c:pt>
@@ -1182,43 +835,103 @@
                   <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>37</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>76</c:v>
                 </c:pt>
-                <c:pt idx="4">
-                  <c:v>1047</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2167</c:v>
+                <c:pt idx="6">
+                  <c:v>88</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>113</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>121</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>152</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>186</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>228</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>312</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>338</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>346</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$J$2:$J$7</c:f>
+              <c:f>Sheet1!$I$18:$I$33</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="16"/>
                 <c:pt idx="0">
                   <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>111</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="2" formatCode="General">
+                  <c:v>653</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>206</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4" formatCode="General">
+                  <c:v>237</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>841</c:v>
                 </c:pt>
-                <c:pt idx="4">
-                  <c:v>35778</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>14437</c:v>
+                <c:pt idx="6" formatCode="General">
+                  <c:v>762</c:v>
+                </c:pt>
+                <c:pt idx="7" formatCode="General">
+                  <c:v>610</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="General">
+                  <c:v>690</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="General">
+                  <c:v>273</c:v>
+                </c:pt>
+                <c:pt idx="10" formatCode="General">
+                  <c:v>841</c:v>
+                </c:pt>
+                <c:pt idx="11" formatCode="General">
+                  <c:v>1331</c:v>
+                </c:pt>
+                <c:pt idx="12" formatCode="General">
+                  <c:v>743</c:v>
+                </c:pt>
+                <c:pt idx="13" formatCode="General">
+                  <c:v>1167</c:v>
+                </c:pt>
+                <c:pt idx="14" formatCode="General">
+                  <c:v>1322</c:v>
+                </c:pt>
+                <c:pt idx="15" formatCode="General">
+                  <c:v>2554</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1227,6 +940,366 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-6828-472B-85A3-62BA7A798480}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Зависимость времени анализа текста от количества страниц</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$H$18:$H$33</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>76</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>88</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>113</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>121</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>152</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>186</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>228</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>312</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>338</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>346</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$J$18:$J$33</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>71</c:v>
+                </c:pt>
+                <c:pt idx="2" formatCode="General">
+                  <c:v>116</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>144</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="General">
+                  <c:v>221</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>295</c:v>
+                </c:pt>
+                <c:pt idx="6" formatCode="General">
+                  <c:v>417</c:v>
+                </c:pt>
+                <c:pt idx="7" formatCode="General">
+                  <c:v>471</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="General">
+                  <c:v>522</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="General">
+                  <c:v>133</c:v>
+                </c:pt>
+                <c:pt idx="10" formatCode="General">
+                  <c:v>325</c:v>
+                </c:pt>
+                <c:pt idx="11" formatCode="General">
+                  <c:v>731</c:v>
+                </c:pt>
+                <c:pt idx="12" formatCode="General">
+                  <c:v>451</c:v>
+                </c:pt>
+                <c:pt idx="13" formatCode="General">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="14" formatCode="General">
+                  <c:v>1544</c:v>
+                </c:pt>
+                <c:pt idx="15" formatCode="General">
+                  <c:v>1049</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-1A68-4D2C-9EF9-5F1FFEA22A09}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Зависимость времени обработки файла от количества страниц</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$H$18:$H$33</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>76</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>88</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>113</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>121</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>152</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>186</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>228</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>312</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>338</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>346</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$K$18:$K$33</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>118</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>182</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>769</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>350</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>458</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1136</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1179</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1081</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1212</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>406</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1166</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2062</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1194</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2167</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2866</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3603</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-1A68-4D2C-9EF9-5F1FFEA22A09}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1245,7 +1318,7 @@
         <c:axId val="672950608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="2200"/>
+          <c:max val="350"/>
           <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -1359,7 +1432,7 @@
         <c:crossAx val="680596160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
-        <c:majorUnit val="400"/>
+        <c:majorUnit val="40"/>
       </c:valAx>
       <c:valAx>
         <c:axId val="680596160"/>
@@ -1495,6 +1568,47 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="8.9465326268178727E-2"/>
+          <c:y val="0.65406514268494931"/>
+          <c:w val="0.83364779874213835"/>
+          <c:h val="0.34287179925050681"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:extLst>
@@ -1539,7 +1653,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -1615,10 +1729,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.17787051618547678"/>
-          <c:y val="0.20916666666666667"/>
-          <c:w val="0.74635170603674539"/>
-          <c:h val="0.61766987459900846"/>
+          <c:x val="0.1344381352630771"/>
+          <c:y val="0.13590662631403008"/>
+          <c:w val="0.81710609262297984"/>
+          <c:h val="0.69092997290820202"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -1666,58 +1780,148 @@
             </c:spPr>
             <c:trendlineType val="linear"/>
             <c:dispRSqr val="0"/>
-            <c:dispEq val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$I$9:$I$14</c:f>
+              <c:f>Sheet1!$J$35:$J$50</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="16"/>
                 <c:pt idx="0">
                   <c:v>10156</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>20818</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="2" formatCode="General">
+                  <c:v>30974</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>42706</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4" formatCode="General">
+                  <c:v>63524</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>108521</c:v>
                 </c:pt>
-                <c:pt idx="4">
-                  <c:v>2717686</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>4120625</c:v>
+                <c:pt idx="6" formatCode="General">
+                  <c:v>139495</c:v>
+                </c:pt>
+                <c:pt idx="7" formatCode="General">
+                  <c:v>151227</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="General">
+                  <c:v>172045</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="General">
+                  <c:v>192665</c:v>
+                </c:pt>
+                <c:pt idx="10" formatCode="General">
+                  <c:v>195506</c:v>
+                </c:pt>
+                <c:pt idx="11" formatCode="General">
+                  <c:v>301186</c:v>
+                </c:pt>
+                <c:pt idx="12" formatCode="General">
+                  <c:v>388171</c:v>
+                </c:pt>
+                <c:pt idx="13" formatCode="General">
+                  <c:v>393400</c:v>
+                </c:pt>
+                <c:pt idx="14" formatCode="General">
+                  <c:v>586065</c:v>
+                </c:pt>
+                <c:pt idx="15" formatCode="General">
+                  <c:v>588906</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$J$9:$J$14</c:f>
+              <c:f>Sheet1!$K$35:$K$50</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="16"/>
                 <c:pt idx="0">
                   <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>71</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="2" formatCode="General">
+                  <c:v>116</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>144</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4" formatCode="General">
+                  <c:v>221</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>295</c:v>
                 </c:pt>
-                <c:pt idx="4">
-                  <c:v>15842</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>37659</c:v>
+                <c:pt idx="6" formatCode="General">
+                  <c:v>417</c:v>
+                </c:pt>
+                <c:pt idx="7" formatCode="General">
+                  <c:v>471</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="General">
+                  <c:v>522</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="General">
+                  <c:v>133</c:v>
+                </c:pt>
+                <c:pt idx="10" formatCode="General">
+                  <c:v>325</c:v>
+                </c:pt>
+                <c:pt idx="11" formatCode="General">
+                  <c:v>451</c:v>
+                </c:pt>
+                <c:pt idx="12" formatCode="General">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="13" formatCode="General">
+                  <c:v>731</c:v>
+                </c:pt>
+                <c:pt idx="14" formatCode="General">
+                  <c:v>1544</c:v>
+                </c:pt>
+                <c:pt idx="15" formatCode="General">
+                  <c:v>1049</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1725,7 +1929,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-3726-4831-A9B0-A0A5776BBDF7}"/>
+              <c16:uniqueId val="{00000001-4F9C-42B1-B68C-201B30E0BA16}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1744,7 +1948,7 @@
         <c:axId val="672950608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="4150000"/>
+          <c:max val="600000"/>
           <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -1858,487 +2062,7 @@
         <c:crossAx val="680596160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
-        <c:majorUnit val="1000000"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="680596160"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-          <c:min val="0"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="ru-RU"/>
-                  <a:t>Время анализа текста, мс</a:t>
-                </a:r>
-                <a:endParaRPr lang="en-US"/>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="0" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="672950608"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr sz="1200"/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1440" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="ru-RU"/>
-              <a:t>Зависимость времени анализа текста от количества символов</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1440" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout>
-        <c:manualLayout>
-          <c:layoutTarget val="inner"/>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="0.15842607174103238"/>
-          <c:y val="0.20916666666666667"/>
-          <c:w val="0.77424059492563435"/>
-          <c:h val="0.61766987459900846"/>
-        </c:manualLayout>
-      </c:layout>
-      <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:v>Зависимость времени извлечения текста от размера файла</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="linear"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="0"/>
-          </c:trendline>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Sheet1!$I$9:$I$12</c:f>
-              <c:numCache>
-                <c:formatCode>0</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>10156</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>20818</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>42706</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>108521</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Sheet1!$J$9:$J$12</c:f>
-              <c:numCache>
-                <c:formatCode>0</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>38</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>71</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>144</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>295</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-4F9C-42B1-B68C-201B30E0BA16}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="672950608"/>
-        <c:axId val="680596160"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="672950608"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-          <c:max val="110000"/>
-          <c:min val="0"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="ru-RU"/>
-                  <a:t>Количество символов, шт.</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="0" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="680596160"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-        <c:majorUnit val="20000"/>
+        <c:majorUnit val="100000"/>
       </c:valAx>
       <c:valAx>
         <c:axId val="680596160"/>
@@ -2393,7 +2117,7 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="1.8083333333333333E-2"/>
+              <c:x val="1.2445495053076083E-2"/>
               <c:y val="0.20916666666666667"/>
             </c:manualLayout>
           </c:layout>
@@ -2639,86 +2363,6 @@
 </cs:colorStyle>
 </file>
 
-<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
-<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -3752,1038 +3396,6 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
-<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
-<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -5304,15 +3916,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>571500</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>23812</xdr:rowOff>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>66676</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>314325</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>100012</xdr:rowOff>
+      <xdr:colOff>1133475</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>27330</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5339,23 +3951,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>628651</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>47624</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>1</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3">
+        <xdr:cNvPr id="7" name="Chart 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{228C7444-78DE-40A8-8AFE-79F4EC6ACFA4}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6713751A-19D8-42DA-8387-8DE9EA4A4F64}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5378,91 +3990,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>542925</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>19049</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="7" name="Chart 6">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6713751A-19D8-42DA-8387-8DE9EA4A4F64}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr>
-          <a:graphicFrameLocks/>
-        </xdr:cNvGraphicFramePr>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>1266825</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>47625</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="8" name="Chart 7">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{04E28E69-32FB-4E58-89E5-F103EF685D31}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr>
-          <a:graphicFrameLocks/>
-        </xdr:cNvGraphicFramePr>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>1257300</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>52</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:row>84</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5483,7 +4019,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -5755,10 +4291,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M14"/>
+  <dimension ref="A1:L67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2:M7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G36" sqref="G36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5770,9 +4306,10 @@
     <col min="5" max="5" width="21.42578125" customWidth="1"/>
     <col min="6" max="6" width="26.140625" customWidth="1"/>
     <col min="7" max="7" width="20" customWidth="1"/>
+    <col min="12" max="12" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -5780,7 +4317,7 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -5792,12 +4329,12 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>5</v>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
       </c>
       <c r="B2" s="2">
         <v>158.12</v>
@@ -5818,24 +4355,15 @@
       <c r="G2" s="1">
         <v>4</v>
       </c>
-      <c r="I2" s="1">
-        <v>4</v>
-      </c>
-      <c r="J2" s="1">
-        <v>80</v>
-      </c>
-      <c r="L2">
-        <f>$B2*1000/$D2</f>
-        <v>1976.5</v>
-      </c>
-      <c r="M2">
-        <f>$C2*1000/$E2</f>
-        <v>267263.15789473685</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>6</v>
+      <c r="I2" s="1"/>
+      <c r="J2" s="4">
+        <f>C2/B2</f>
+        <v>64.229698962813046</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
       </c>
       <c r="B3" s="2">
         <v>293.79000000000002</v>
@@ -5850,230 +4378,900 @@
         <v>71</v>
       </c>
       <c r="F3" s="1">
-        <f t="shared" ref="F3:F7" si="0">$D3+$E3</f>
+        <f>$D3+$E3</f>
         <v>182</v>
       </c>
       <c r="G3" s="1">
         <v>8</v>
       </c>
-      <c r="I3" s="1">
+      <c r="I3" s="1"/>
+      <c r="J3" s="4">
+        <f t="shared" ref="J3:J17" si="0">C3/B3</f>
+        <v>70.860138193948046</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>427.51</v>
+      </c>
+      <c r="C4">
+        <v>30974</v>
+      </c>
+      <c r="D4">
+        <v>653</v>
+      </c>
+      <c r="E4">
+        <v>116</v>
+      </c>
+      <c r="F4" s="1">
+        <f>$D4+$E4</f>
+        <v>769</v>
+      </c>
+      <c r="G4" s="1">
+        <v>12</v>
+      </c>
+      <c r="I4" s="1"/>
+      <c r="J4" s="4">
+        <f t="shared" si="0"/>
+        <v>72.452106383476405</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2">
+        <v>702.12</v>
+      </c>
+      <c r="C5" s="1">
+        <v>42706</v>
+      </c>
+      <c r="D5" s="1">
+        <v>206</v>
+      </c>
+      <c r="E5" s="1">
+        <v>144</v>
+      </c>
+      <c r="F5" s="1">
+        <f>$D5+$E5</f>
+        <v>350</v>
+      </c>
+      <c r="G5" s="1">
+        <v>37</v>
+      </c>
+      <c r="I5" s="1"/>
+      <c r="J5" s="4">
+        <f t="shared" si="0"/>
+        <v>60.824360508175239</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>939.52</v>
+      </c>
+      <c r="C6">
+        <v>63524</v>
+      </c>
+      <c r="D6">
+        <v>237</v>
+      </c>
+      <c r="E6">
+        <v>221</v>
+      </c>
+      <c r="F6" s="1">
+        <f>$D6+$E6</f>
+        <v>458</v>
+      </c>
+      <c r="G6" s="1">
+        <v>45</v>
+      </c>
+      <c r="I6" s="1"/>
+      <c r="J6" s="4">
+        <f t="shared" si="0"/>
+        <v>67.613249318801095</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2">
+        <v>1654.55</v>
+      </c>
+      <c r="C7" s="1">
+        <v>108521</v>
+      </c>
+      <c r="D7" s="1">
+        <v>841</v>
+      </c>
+      <c r="E7" s="1">
+        <v>295</v>
+      </c>
+      <c r="F7" s="1">
+        <f>$D7+$E7</f>
+        <v>1136</v>
+      </c>
+      <c r="G7" s="1">
+        <v>76</v>
+      </c>
+      <c r="I7" s="1"/>
+      <c r="J7" s="4">
+        <f t="shared" si="0"/>
+        <v>65.589435193859359</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>1905.22</v>
+      </c>
+      <c r="C8">
+        <v>139495</v>
+      </c>
+      <c r="D8">
+        <v>762</v>
+      </c>
+      <c r="E8">
+        <v>417</v>
+      </c>
+      <c r="F8" s="1">
+        <f>$D8+$E8</f>
+        <v>1179</v>
+      </c>
+      <c r="G8" s="1">
+        <v>88</v>
+      </c>
+      <c r="J8" s="4">
+        <f t="shared" si="0"/>
+        <v>73.217266247467478</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9">
         <v>8</v>
       </c>
-      <c r="J3" s="1">
+      <c r="B9">
+        <v>2140.2600000000002</v>
+      </c>
+      <c r="C9">
+        <v>151227</v>
+      </c>
+      <c r="D9">
+        <v>610</v>
+      </c>
+      <c r="E9">
+        <v>471</v>
+      </c>
+      <c r="F9" s="1">
+        <f>$D9+$E9</f>
+        <v>1081</v>
+      </c>
+      <c r="G9" s="1">
+        <v>113</v>
+      </c>
+      <c r="I9" s="1"/>
+      <c r="J9" s="4">
+        <f t="shared" si="0"/>
+        <v>70.658237784194441</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>2418.71</v>
+      </c>
+      <c r="C10">
+        <v>172045</v>
+      </c>
+      <c r="D10">
+        <v>690</v>
+      </c>
+      <c r="E10">
+        <v>522</v>
+      </c>
+      <c r="F10" s="1">
+        <f>$D10+$E10</f>
+        <v>1212</v>
+      </c>
+      <c r="G10" s="1">
+        <v>121</v>
+      </c>
+      <c r="I10" s="1"/>
+      <c r="J10" s="4">
+        <f t="shared" si="0"/>
+        <v>71.130892087104286</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>2700.42</v>
+      </c>
+      <c r="C11">
+        <v>192665</v>
+      </c>
+      <c r="D11">
+        <v>273</v>
+      </c>
+      <c r="E11">
+        <v>133</v>
+      </c>
+      <c r="F11" s="1">
+        <f>$D11+$E11</f>
+        <v>406</v>
+      </c>
+      <c r="G11" s="1">
+        <v>152</v>
+      </c>
+      <c r="I11" s="1"/>
+      <c r="J11" s="4">
+        <f t="shared" si="0"/>
+        <v>71.346309092659652</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>4209.57</v>
+      </c>
+      <c r="C12">
+        <v>301186</v>
+      </c>
+      <c r="D12">
+        <v>743</v>
+      </c>
+      <c r="E12">
+        <v>451</v>
+      </c>
+      <c r="F12" s="1">
+        <f>$D12+$E12</f>
+        <v>1194</v>
+      </c>
+      <c r="G12" s="1">
+        <v>228</v>
+      </c>
+      <c r="I12" s="1"/>
+      <c r="J12" s="4">
+        <f t="shared" si="0"/>
+        <v>71.547925322538887</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>4769.96</v>
+      </c>
+      <c r="C13">
+        <v>393400</v>
+      </c>
+      <c r="D13">
+        <v>1331</v>
+      </c>
+      <c r="E13">
+        <v>731</v>
+      </c>
+      <c r="F13" s="1">
+        <f>$D13+$E13</f>
+        <v>2062</v>
+      </c>
+      <c r="G13" s="1">
+        <v>186</v>
+      </c>
+      <c r="I13" s="1"/>
+      <c r="J13" s="4">
+        <f t="shared" si="0"/>
+        <v>82.474486159213072</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>6046.34</v>
+      </c>
+      <c r="C14">
+        <v>195506</v>
+      </c>
+      <c r="D14">
+        <v>841</v>
+      </c>
+      <c r="E14">
+        <v>325</v>
+      </c>
+      <c r="F14" s="1">
+        <f>$D14+$E14</f>
+        <v>1166</v>
+      </c>
+      <c r="G14" s="1">
+        <v>160</v>
+      </c>
+      <c r="I14" s="1"/>
+      <c r="J14" s="4">
+        <f t="shared" si="0"/>
+        <v>32.334602420637935</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>7286.54</v>
+      </c>
+      <c r="C15">
+        <v>586065</v>
+      </c>
+      <c r="D15">
+        <v>1322</v>
+      </c>
+      <c r="E15">
+        <v>1544</v>
+      </c>
+      <c r="F15" s="1">
+        <f>$D15+$E15</f>
+        <v>2866</v>
+      </c>
+      <c r="G15" s="1">
+        <v>338</v>
+      </c>
+      <c r="J15" s="4">
+        <f t="shared" si="0"/>
+        <v>80.431178584074203</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>8746.08</v>
+      </c>
+      <c r="C16">
+        <v>388171</v>
+      </c>
+      <c r="D16">
+        <v>1167</v>
+      </c>
+      <c r="E16">
+        <v>1000</v>
+      </c>
+      <c r="F16" s="1">
+        <f>$D16+$E16</f>
+        <v>2167</v>
+      </c>
+      <c r="G16" s="1">
+        <v>312</v>
+      </c>
+      <c r="J16" s="4">
+        <f t="shared" si="0"/>
+        <v>44.38228326290178</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>10575.51</v>
+      </c>
+      <c r="C17">
+        <v>588906</v>
+      </c>
+      <c r="D17">
+        <v>2554</v>
+      </c>
+      <c r="E17">
+        <v>1049</v>
+      </c>
+      <c r="F17" s="1">
+        <f>$D17+$E17</f>
+        <v>3603</v>
+      </c>
+      <c r="G17" s="1">
+        <v>346</v>
+      </c>
+      <c r="J17" s="4">
+        <f t="shared" si="0"/>
+        <v>55.685825080776247</v>
+      </c>
+      <c r="L17" s="3"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B18" s="2"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1">
+        <v>4</v>
+      </c>
+      <c r="I18" s="1">
+        <v>80</v>
+      </c>
+      <c r="J18" s="1">
+        <v>38</v>
+      </c>
+      <c r="K18" s="1">
+        <f>$I18+$J18</f>
+        <v>118</v>
+      </c>
+      <c r="L18" s="1"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B19" s="2"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1">
+        <v>8</v>
+      </c>
+      <c r="I19" s="1">
         <v>111</v>
       </c>
-      <c r="L3">
-        <f t="shared" ref="L3:L7" si="1">$B3*1000/$D3</f>
-        <v>2646.7567567567567</v>
-      </c>
-      <c r="M3">
-        <f t="shared" ref="M3:M7" si="2">$C3*1000/$E3</f>
-        <v>293211.26760563382</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="2">
-        <v>702.12</v>
-      </c>
-      <c r="C4" s="1">
+      <c r="J19" s="1">
+        <v>71</v>
+      </c>
+      <c r="K19" s="1">
+        <f>$I19+$J19</f>
+        <v>182</v>
+      </c>
+      <c r="L19" s="1"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H20" s="1">
+        <v>12</v>
+      </c>
+      <c r="I20">
+        <v>653</v>
+      </c>
+      <c r="J20">
+        <v>116</v>
+      </c>
+      <c r="K20" s="1">
+        <f>$I20+$J20</f>
+        <v>769</v>
+      </c>
+      <c r="L20" s="1"/>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H21" s="1">
+        <v>37</v>
+      </c>
+      <c r="I21" s="1">
+        <v>206</v>
+      </c>
+      <c r="J21" s="1">
+        <v>144</v>
+      </c>
+      <c r="K21" s="1">
+        <f>$I21+$J21</f>
+        <v>350</v>
+      </c>
+      <c r="L21" s="1"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H22" s="1">
+        <v>45</v>
+      </c>
+      <c r="I22">
+        <v>237</v>
+      </c>
+      <c r="J22">
+        <v>221</v>
+      </c>
+      <c r="K22" s="1">
+        <f>$I22+$J22</f>
+        <v>458</v>
+      </c>
+      <c r="L22" s="1"/>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H23" s="1">
+        <v>76</v>
+      </c>
+      <c r="I23" s="1">
+        <v>841</v>
+      </c>
+      <c r="J23" s="1">
+        <v>295</v>
+      </c>
+      <c r="K23" s="1">
+        <f>$I23+$J23</f>
+        <v>1136</v>
+      </c>
+      <c r="L23" s="1"/>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H24" s="1">
+        <v>88</v>
+      </c>
+      <c r="I24">
+        <v>762</v>
+      </c>
+      <c r="J24">
+        <v>417</v>
+      </c>
+      <c r="K24" s="1">
+        <f>$I24+$J24</f>
+        <v>1179</v>
+      </c>
+      <c r="L24" s="1"/>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H25" s="1">
+        <v>113</v>
+      </c>
+      <c r="I25">
+        <v>610</v>
+      </c>
+      <c r="J25">
+        <v>471</v>
+      </c>
+      <c r="K25" s="1">
+        <f>$I25+$J25</f>
+        <v>1081</v>
+      </c>
+      <c r="L25" s="1"/>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H26" s="1">
+        <v>121</v>
+      </c>
+      <c r="I26">
+        <v>690</v>
+      </c>
+      <c r="J26">
+        <v>522</v>
+      </c>
+      <c r="K26" s="1">
+        <f>$I26+$J26</f>
+        <v>1212</v>
+      </c>
+      <c r="L26" s="1"/>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H27" s="1">
+        <v>152</v>
+      </c>
+      <c r="I27">
+        <v>273</v>
+      </c>
+      <c r="J27">
+        <v>133</v>
+      </c>
+      <c r="K27" s="1">
+        <f>$I27+$J27</f>
+        <v>406</v>
+      </c>
+      <c r="L27" s="1"/>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H28" s="1">
+        <v>160</v>
+      </c>
+      <c r="I28">
+        <v>841</v>
+      </c>
+      <c r="J28">
+        <v>325</v>
+      </c>
+      <c r="K28" s="1">
+        <f>$I28+$J28</f>
+        <v>1166</v>
+      </c>
+      <c r="L28" s="1"/>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H29" s="1">
+        <v>186</v>
+      </c>
+      <c r="I29">
+        <v>1331</v>
+      </c>
+      <c r="J29">
+        <v>731</v>
+      </c>
+      <c r="K29" s="1">
+        <f>$I29+$J29</f>
+        <v>2062</v>
+      </c>
+      <c r="L29" s="1"/>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H30" s="1">
+        <v>228</v>
+      </c>
+      <c r="I30">
+        <v>743</v>
+      </c>
+      <c r="J30">
+        <v>451</v>
+      </c>
+      <c r="K30" s="1">
+        <f>$I30+$J30</f>
+        <v>1194</v>
+      </c>
+      <c r="L30" s="1"/>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H31" s="1">
+        <v>312</v>
+      </c>
+      <c r="I31">
+        <v>1167</v>
+      </c>
+      <c r="J31">
+        <v>1000</v>
+      </c>
+      <c r="K31" s="1">
+        <f>$I31+$J31</f>
+        <v>2167</v>
+      </c>
+      <c r="L31" s="1"/>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H32" s="1">
+        <v>338</v>
+      </c>
+      <c r="I32">
+        <v>1322</v>
+      </c>
+      <c r="J32">
+        <v>1544</v>
+      </c>
+      <c r="K32" s="1">
+        <f>$I32+$J32</f>
+        <v>2866</v>
+      </c>
+      <c r="L32" s="1"/>
+    </row>
+    <row r="33" spans="8:12" x14ac:dyDescent="0.25">
+      <c r="H33" s="1">
+        <v>346</v>
+      </c>
+      <c r="I33">
+        <v>2554</v>
+      </c>
+      <c r="J33">
+        <v>1049</v>
+      </c>
+      <c r="K33" s="1">
+        <f>$I33+$J33</f>
+        <v>3603</v>
+      </c>
+      <c r="L33" s="1"/>
+    </row>
+    <row r="35" spans="8:12" x14ac:dyDescent="0.25">
+      <c r="J35" s="1">
+        <v>10156</v>
+      </c>
+      <c r="K35" s="1">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="36" spans="8:12" x14ac:dyDescent="0.25">
+      <c r="J36" s="1">
+        <v>20818</v>
+      </c>
+      <c r="K36" s="1">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="37" spans="8:12" x14ac:dyDescent="0.25">
+      <c r="J37">
+        <v>30974</v>
+      </c>
+      <c r="K37">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="38" spans="8:12" x14ac:dyDescent="0.25">
+      <c r="J38" s="1">
         <v>42706</v>
       </c>
-      <c r="D4" s="1">
-        <v>206</v>
-      </c>
-      <c r="E4" s="1">
+      <c r="K38" s="1">
         <v>144</v>
       </c>
-      <c r="F4" s="1">
-        <f t="shared" si="0"/>
-        <v>350</v>
-      </c>
-      <c r="G4" s="1">
+    </row>
+    <row r="39" spans="8:12" x14ac:dyDescent="0.25">
+      <c r="J39">
+        <v>63524</v>
+      </c>
+      <c r="K39">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="40" spans="8:12" x14ac:dyDescent="0.25">
+      <c r="J40" s="1">
+        <v>108521</v>
+      </c>
+      <c r="K40" s="1">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="41" spans="8:12" x14ac:dyDescent="0.25">
+      <c r="J41">
+        <v>139495</v>
+      </c>
+      <c r="K41">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="42" spans="8:12" x14ac:dyDescent="0.25">
+      <c r="J42">
+        <v>151227</v>
+      </c>
+      <c r="K42">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="43" spans="8:12" x14ac:dyDescent="0.25">
+      <c r="J43">
+        <v>172045</v>
+      </c>
+      <c r="K43">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="44" spans="8:12" x14ac:dyDescent="0.25">
+      <c r="J44">
+        <v>192665</v>
+      </c>
+      <c r="K44">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="45" spans="8:12" x14ac:dyDescent="0.25">
+      <c r="J45">
+        <v>195506</v>
+      </c>
+      <c r="K45">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="46" spans="8:12" x14ac:dyDescent="0.25">
+      <c r="J46">
+        <v>301186</v>
+      </c>
+      <c r="K46">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="47" spans="8:12" x14ac:dyDescent="0.25">
+      <c r="J47">
+        <v>388171</v>
+      </c>
+      <c r="K47">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="48" spans="8:12" x14ac:dyDescent="0.25">
+      <c r="J48">
+        <v>393400</v>
+      </c>
+      <c r="K48">
+        <v>731</v>
+      </c>
+    </row>
+    <row r="49" spans="10:11" x14ac:dyDescent="0.25">
+      <c r="J49">
+        <v>586065</v>
+      </c>
+      <c r="K49">
+        <v>1544</v>
+      </c>
+    </row>
+    <row r="50" spans="10:11" x14ac:dyDescent="0.25">
+      <c r="J50">
+        <v>588906</v>
+      </c>
+      <c r="K50">
+        <v>1049</v>
+      </c>
+    </row>
+    <row r="52" spans="10:11" x14ac:dyDescent="0.25">
+      <c r="J52" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="53" spans="10:11" x14ac:dyDescent="0.25">
+      <c r="J53" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="54" spans="10:11" x14ac:dyDescent="0.25">
+      <c r="J54" s="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="55" spans="10:11" x14ac:dyDescent="0.25">
+      <c r="J55" s="1">
         <v>37</v>
       </c>
-      <c r="I4" s="1">
-        <v>37</v>
-      </c>
-      <c r="J4" s="1">
-        <v>206</v>
-      </c>
-      <c r="L4">
-        <f t="shared" si="1"/>
-        <v>3408.3495145631068</v>
-      </c>
-      <c r="M4">
-        <f t="shared" si="2"/>
-        <v>296569.44444444444</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="2">
-        <v>1654.55</v>
-      </c>
-      <c r="C5" s="1">
-        <v>108521</v>
-      </c>
-      <c r="D5" s="1">
-        <v>841</v>
-      </c>
-      <c r="E5" s="1">
-        <v>295</v>
-      </c>
-      <c r="F5" s="1">
-        <f t="shared" si="0"/>
-        <v>1136</v>
-      </c>
-      <c r="G5" s="1">
+    </row>
+    <row r="56" spans="10:11" x14ac:dyDescent="0.25">
+      <c r="J56" s="1">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="57" spans="10:11" x14ac:dyDescent="0.25">
+      <c r="J57" s="1">
         <v>76</v>
       </c>
-      <c r="I5" s="1">
-        <v>76</v>
-      </c>
-      <c r="J5" s="1">
-        <v>841</v>
-      </c>
-      <c r="L5">
-        <f t="shared" si="1"/>
-        <v>1967.360285374554</v>
-      </c>
-      <c r="M5">
-        <f t="shared" si="2"/>
-        <v>367867.79661016952</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="2">
-        <v>9738.32</v>
-      </c>
-      <c r="C6" s="1">
-        <v>4120625</v>
-      </c>
-      <c r="D6" s="1">
-        <v>14437</v>
-      </c>
-      <c r="E6" s="1">
-        <v>37659</v>
-      </c>
-      <c r="F6" s="1">
-        <f t="shared" si="0"/>
-        <v>52096</v>
-      </c>
-      <c r="G6" s="1">
-        <v>2167</v>
-      </c>
-      <c r="I6" s="1">
-        <v>1047</v>
-      </c>
-      <c r="J6" s="1">
-        <v>35778</v>
-      </c>
-      <c r="L6">
-        <f t="shared" si="1"/>
-        <v>674.53903165477595</v>
-      </c>
-      <c r="M6">
-        <f t="shared" si="2"/>
-        <v>109419.39509811731</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="2">
-        <v>42533.51</v>
-      </c>
-      <c r="C7" s="1">
-        <v>2717686</v>
-      </c>
-      <c r="D7" s="1">
-        <v>35778</v>
-      </c>
-      <c r="E7" s="1">
-        <v>15842</v>
-      </c>
-      <c r="F7" s="1">
-        <f t="shared" si="0"/>
-        <v>51620</v>
-      </c>
-      <c r="G7" s="1">
-        <v>1047</v>
-      </c>
-      <c r="I7" s="1">
-        <v>2167</v>
-      </c>
-      <c r="J7" s="1">
-        <v>14437</v>
-      </c>
-      <c r="L7">
-        <f t="shared" si="1"/>
-        <v>1188.8174297054056</v>
-      </c>
-      <c r="M7">
-        <f t="shared" si="2"/>
-        <v>171549.4255775786</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="I9" s="1">
-        <v>10156</v>
-      </c>
-      <c r="J9" s="1">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="I10" s="1">
-        <v>20818</v>
-      </c>
-      <c r="J10" s="1">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="I11" s="1">
-        <v>42706</v>
-      </c>
-      <c r="J11" s="1">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="I12" s="1">
-        <v>108521</v>
-      </c>
-      <c r="J12" s="1">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="I13" s="1">
-        <v>2717686</v>
-      </c>
-      <c r="J13" s="1">
-        <v>15842</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="I14" s="1">
-        <v>4120625</v>
-      </c>
-      <c r="J14" s="1">
-        <v>37659</v>
+    </row>
+    <row r="58" spans="10:11" x14ac:dyDescent="0.25">
+      <c r="J58" s="1">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="59" spans="10:11" x14ac:dyDescent="0.25">
+      <c r="J59" s="1">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="60" spans="10:11" x14ac:dyDescent="0.25">
+      <c r="J60" s="1">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="61" spans="10:11" x14ac:dyDescent="0.25">
+      <c r="J61" s="1">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="62" spans="10:11" x14ac:dyDescent="0.25">
+      <c r="J62" s="1">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="63" spans="10:11" x14ac:dyDescent="0.25">
+      <c r="J63" s="1">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="64" spans="10:11" x14ac:dyDescent="0.25">
+      <c r="J64" s="1">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="65" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J65" s="1">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="66" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J66" s="1">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="67" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J67" s="1">
+        <v>346</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="I9:J14">
-    <sortCondition ref="I9"/>
+  <sortState ref="H18:K33">
+    <sortCondition ref="H18"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>